<commit_message>
Imports Calls, Dossiers and Fiches
</commit_message>
<xml_diff>
--- a/storage/excel/TV_Dossiers.xlsx
+++ b/storage/excel/TV_Dossiers.xlsx
@@ -2154,7 +2154,7 @@
   <dimension ref="A1:J341"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2187,10 +2187,10 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>